<commit_message>
Add analyses, internal consistency begin, and start paper.
</commit_message>
<xml_diff>
--- a/meta_spreadsheet.xlsx
+++ b/meta_spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\Desktop\OneDrive - Florida State University\Florida State University\Research Projects\erp_suicide_meta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Austin\Desktop\OneDrive - Florida State University\Florida State University\Research Projects\meta_suicide_erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="390" documentId="8_{AE6EE886-186C-438A-A3D8-7543467F2F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8E6750FF-024D-44B2-A4CD-E6A0E9A37F7D}"/>
+  <xr:revisionPtr revIDLastSave="391" documentId="8_{AE6EE886-186C-438A-A3D8-7543467F2F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77265382-3ABD-46E9-A3B5-54702412A994}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="3" xr2:uid="{FF3FF6FC-0C5E-41B5-84E2-C5FF2C3F66C7}"/>
   </bookViews>
@@ -2325,9 +2325,6 @@
     <t>Latent No-Go P3</t>
   </si>
   <si>
-    <t>Latnet Go P3</t>
-  </si>
-  <si>
     <t>P2</t>
   </si>
   <si>
@@ -2698,6 +2695,9 @@
   </si>
   <si>
     <t>2019b</t>
+  </si>
+  <si>
+    <t>Latent Go P3</t>
   </si>
 </sst>
 </file>
@@ -8460,10 +8460,10 @@
   <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8526,7 +8526,7 @@
         <v>18</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.45">
@@ -8564,7 +8564,7 @@
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.45">
@@ -8602,7 +8602,7 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.45">
@@ -8640,7 +8640,7 @@
         <v>3</v>
       </c>
       <c r="P4" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.45">
@@ -8678,7 +8678,7 @@
         <v>4</v>
       </c>
       <c r="P5" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.45">
@@ -8838,7 +8838,7 @@
         <v>5</v>
       </c>
       <c r="P10" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
@@ -8879,7 +8879,7 @@
         <v>7</v>
       </c>
       <c r="P11" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
@@ -8946,7 +8946,7 @@
         <v>6</v>
       </c>
       <c r="P13" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
@@ -9048,7 +9048,7 @@
         <v>8</v>
       </c>
       <c r="P16" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.45">
@@ -9086,7 +9086,7 @@
         <v>9</v>
       </c>
       <c r="P17" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.45">
@@ -9156,7 +9156,7 @@
         <v>11</v>
       </c>
       <c r="P19" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.45">
@@ -9194,7 +9194,7 @@
         <v>10</v>
       </c>
       <c r="P20" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="21" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -9284,13 +9284,13 @@
         <v>1</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="O23" s="6">
         <v>12</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="24" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
@@ -9459,7 +9459,7 @@
         <v>13</v>
       </c>
       <c r="P28" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.45">
@@ -9497,7 +9497,7 @@
         <v>14</v>
       </c>
       <c r="P29" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
@@ -9605,7 +9605,7 @@
         <v>15</v>
       </c>
       <c r="P32" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.45">
@@ -9643,7 +9643,7 @@
         <v>16</v>
       </c>
       <c r="P33" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.45">
@@ -9704,7 +9704,7 @@
         <v>17</v>
       </c>
       <c r="P35" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.45">
@@ -9864,7 +9864,7 @@
         <v>18</v>
       </c>
       <c r="P40" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.45">
@@ -9905,7 +9905,7 @@
         <v>19</v>
       </c>
       <c r="P41" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.45">
@@ -9946,7 +9946,7 @@
         <v>20</v>
       </c>
       <c r="P42" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.45">
@@ -10108,7 +10108,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B48" t="s">
         <v>417</v>
@@ -10123,7 +10123,7 @@
         <v>346</v>
       </c>
       <c r="F48" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G48" t="s">
         <v>688</v>
@@ -10138,18 +10138,18 @@
         <v>688</v>
       </c>
       <c r="L48" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="O48">
         <v>21</v>
       </c>
       <c r="P48" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="B49" t="s">
         <v>475</v>
@@ -10161,10 +10161,10 @@
         <v>1983</v>
       </c>
       <c r="E49" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F49" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G49" t="s">
         <v>36</v>
@@ -10179,7 +10179,7 @@
         <v>36</v>
       </c>
       <c r="P49" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.45">
@@ -10190,10 +10190,10 @@
         <v>43</v>
       </c>
       <c r="D50" t="s">
+        <v>854</v>
+      </c>
+      <c r="F50" t="s">
         <v>855</v>
-      </c>
-      <c r="F50" t="s">
-        <v>856</v>
       </c>
       <c r="G50" t="s">
         <v>688</v>
@@ -10219,10 +10219,10 @@
         <v>43</v>
       </c>
       <c r="D51" t="s">
+        <v>854</v>
+      </c>
+      <c r="F51" t="s">
         <v>855</v>
-      </c>
-      <c r="F51" t="s">
-        <v>856</v>
       </c>
       <c r="G51" t="s">
         <v>688</v>
@@ -10254,9 +10254,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E90853A-A82C-4185-AE1B-AC3373DE1028}">
   <dimension ref="A1:AE115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10286,7 +10286,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>11</v>
@@ -10310,7 +10310,7 @@
         <v>32</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>19</v>
@@ -10367,13 +10367,13 @@
         <v>711</v>
       </c>
       <c r="AC1" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>852</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>853</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="2" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -10381,10 +10381,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C2" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -10446,10 +10446,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -10511,10 +10511,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C4" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -10576,10 +10576,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C5" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -10641,10 +10641,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -10706,10 +10706,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C7" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -10771,10 +10771,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C8" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -10836,10 +10836,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C9" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -10901,10 +10901,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C10" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -10966,10 +10966,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C11" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -11031,10 +11031,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C12" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D12">
         <v>11</v>
@@ -11096,10 +11096,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C13" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -11161,10 +11161,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C14" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -11226,10 +11226,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
+        <v>883</v>
+      </c>
+      <c r="C15" t="s">
         <v>884</v>
-      </c>
-      <c r="C15" t="s">
-        <v>885</v>
       </c>
       <c r="D15">
         <v>14</v>
@@ -11313,10 +11313,10 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
+        <v>883</v>
+      </c>
+      <c r="C16" t="s">
         <v>884</v>
-      </c>
-      <c r="C16" t="s">
-        <v>885</v>
       </c>
       <c r="D16">
         <v>15</v>
@@ -11400,10 +11400,10 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
+        <v>883</v>
+      </c>
+      <c r="C17" t="s">
         <v>884</v>
-      </c>
-      <c r="C17" t="s">
-        <v>885</v>
       </c>
       <c r="D17">
         <v>16</v>
@@ -11487,10 +11487,10 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
+        <v>883</v>
+      </c>
+      <c r="C18" t="s">
         <v>884</v>
-      </c>
-      <c r="C18" t="s">
-        <v>885</v>
       </c>
       <c r="D18">
         <v>17</v>
@@ -11574,10 +11574,10 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>883</v>
+      </c>
+      <c r="C19" t="s">
         <v>884</v>
-      </c>
-      <c r="C19" t="s">
-        <v>885</v>
       </c>
       <c r="D19">
         <v>18</v>
@@ -11661,10 +11661,10 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
+        <v>883</v>
+      </c>
+      <c r="C20" t="s">
         <v>884</v>
-      </c>
-      <c r="C20" t="s">
-        <v>885</v>
       </c>
       <c r="D20">
         <v>19</v>
@@ -11748,10 +11748,10 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>883</v>
+      </c>
+      <c r="C21" t="s">
         <v>884</v>
-      </c>
-      <c r="C21" t="s">
-        <v>885</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -11835,10 +11835,10 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
+        <v>883</v>
+      </c>
+      <c r="C22" t="s">
         <v>884</v>
-      </c>
-      <c r="C22" t="s">
-        <v>885</v>
       </c>
       <c r="D22">
         <v>21</v>
@@ -11922,10 +11922,10 @@
         <v>2</v>
       </c>
       <c r="B23" t="s">
+        <v>883</v>
+      </c>
+      <c r="C23" t="s">
         <v>884</v>
-      </c>
-      <c r="C23" t="s">
-        <v>885</v>
       </c>
       <c r="D23">
         <v>22</v>
@@ -12009,10 +12009,10 @@
         <v>2</v>
       </c>
       <c r="B24" t="s">
+        <v>883</v>
+      </c>
+      <c r="C24" t="s">
         <v>884</v>
-      </c>
-      <c r="C24" t="s">
-        <v>885</v>
       </c>
       <c r="D24">
         <v>23</v>
@@ -12096,10 +12096,10 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>883</v>
+      </c>
+      <c r="C25" t="s">
         <v>884</v>
-      </c>
-      <c r="C25" t="s">
-        <v>885</v>
       </c>
       <c r="D25">
         <v>24</v>
@@ -12183,10 +12183,10 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>883</v>
+      </c>
+      <c r="C26" t="s">
         <v>884</v>
-      </c>
-      <c r="C26" t="s">
-        <v>885</v>
       </c>
       <c r="D26">
         <v>25</v>
@@ -12228,7 +12228,7 @@
         <v>724</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>762</v>
+        <v>886</v>
       </c>
       <c r="R26">
         <v>1.04</v>
@@ -12270,7 +12270,7 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C27">
         <v>2019</v>
@@ -12300,10 +12300,10 @@
         <v>748</v>
       </c>
       <c r="P27" t="s">
+        <v>762</v>
+      </c>
+      <c r="Q27" t="s">
         <v>763</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>764</v>
       </c>
       <c r="V27">
         <v>56</v>
@@ -12335,7 +12335,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C28">
         <v>2019</v>
@@ -12365,10 +12365,10 @@
         <v>748</v>
       </c>
       <c r="P28" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="Q28" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="V28">
         <v>56</v>
@@ -12400,7 +12400,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C29">
         <v>2019</v>
@@ -12430,10 +12430,10 @@
         <v>748</v>
       </c>
       <c r="P29" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="Q29" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="V29">
         <v>56</v>
@@ -12465,7 +12465,7 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C30">
         <v>2019</v>
@@ -12498,7 +12498,7 @@
         <v>724</v>
       </c>
       <c r="Q30" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="V30">
         <v>56</v>
@@ -12530,7 +12530,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C31">
         <v>2019</v>
@@ -12563,7 +12563,7 @@
         <v>724</v>
       </c>
       <c r="Q31" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="V31">
         <v>56</v>
@@ -12595,7 +12595,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C32">
         <v>2019</v>
@@ -12628,7 +12628,7 @@
         <v>724</v>
       </c>
       <c r="Q32" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="V32">
         <v>56</v>
@@ -12660,7 +12660,7 @@
         <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C33">
         <v>2019</v>
@@ -12693,7 +12693,7 @@
         <v>731</v>
       </c>
       <c r="Q33" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="V33">
         <v>56</v>
@@ -12725,7 +12725,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C34">
         <v>2019</v>
@@ -12758,7 +12758,7 @@
         <v>731</v>
       </c>
       <c r="Q34" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="V34">
         <v>56</v>
@@ -12790,7 +12790,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C35">
         <v>2019</v>
@@ -12823,7 +12823,7 @@
         <v>731</v>
       </c>
       <c r="Q35" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="V35">
         <v>56</v>
@@ -12855,7 +12855,7 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C36">
         <v>2019</v>
@@ -12888,7 +12888,7 @@
         <v>724</v>
       </c>
       <c r="Q36" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="V36">
         <v>56</v>
@@ -12920,7 +12920,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C37">
         <v>2019</v>
@@ -12953,7 +12953,7 @@
         <v>724</v>
       </c>
       <c r="Q37" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="V37">
         <v>56</v>
@@ -12985,7 +12985,7 @@
         <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C38">
         <v>2019</v>
@@ -13018,7 +13018,7 @@
         <v>724</v>
       </c>
       <c r="Q38" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="V38">
         <v>56</v>
@@ -13050,7 +13050,7 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C39">
         <v>2019</v>
@@ -13083,7 +13083,7 @@
         <v>704</v>
       </c>
       <c r="Q39" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="V39">
         <v>56</v>
@@ -13115,7 +13115,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C40">
         <v>2019</v>
@@ -13148,7 +13148,7 @@
         <v>704</v>
       </c>
       <c r="Q40" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="V40">
         <v>56</v>
@@ -13180,7 +13180,7 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C41">
         <v>2019</v>
@@ -13213,7 +13213,7 @@
         <v>704</v>
       </c>
       <c r="Q41" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="V41">
         <v>56</v>
@@ -13245,7 +13245,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C42">
         <v>2019</v>
@@ -13278,7 +13278,7 @@
         <v>704</v>
       </c>
       <c r="Q42" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="V42">
         <v>56</v>
@@ -13310,7 +13310,7 @@
         <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C43">
         <v>2019</v>
@@ -13343,7 +13343,7 @@
         <v>704</v>
       </c>
       <c r="Q43" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="V43">
         <v>56</v>
@@ -13375,7 +13375,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C44">
         <v>2019</v>
@@ -13408,7 +13408,7 @@
         <v>704</v>
       </c>
       <c r="Q44" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="V44">
         <v>56</v>
@@ -13440,7 +13440,7 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C45">
         <v>2019</v>
@@ -13473,7 +13473,7 @@
         <v>724</v>
       </c>
       <c r="Q45" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="V45">
         <v>56</v>
@@ -13505,7 +13505,7 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C46">
         <v>2019</v>
@@ -13538,7 +13538,7 @@
         <v>724</v>
       </c>
       <c r="Q46" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="V46">
         <v>56</v>
@@ -13570,7 +13570,7 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C47">
         <v>2019</v>
@@ -13603,7 +13603,7 @@
         <v>724</v>
       </c>
       <c r="Q47" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="V47">
         <v>56</v>
@@ -13635,7 +13635,7 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C48">
         <v>2019</v>
@@ -13668,7 +13668,7 @@
         <v>724</v>
       </c>
       <c r="Q48" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="V48">
         <v>56</v>
@@ -13700,7 +13700,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C49">
         <v>2019</v>
@@ -13733,7 +13733,7 @@
         <v>724</v>
       </c>
       <c r="Q49" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="V49">
         <v>56</v>
@@ -13765,7 +13765,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C50">
         <v>2019</v>
@@ -13798,7 +13798,7 @@
         <v>724</v>
       </c>
       <c r="Q50" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="V50">
         <v>56</v>
@@ -13830,7 +13830,7 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C51">
         <v>2019</v>
@@ -13875,7 +13875,7 @@
         <v>704</v>
       </c>
       <c r="Q51" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="V51">
         <f>K51+L51</f>
@@ -13908,7 +13908,7 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C52">
         <v>2019</v>
@@ -13953,7 +13953,7 @@
         <v>704</v>
       </c>
       <c r="Q52" s="2" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="R52">
         <v>4.9800000000000004</v>
@@ -13995,7 +13995,7 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C53">
         <v>2019</v>
@@ -14040,7 +14040,7 @@
         <v>704</v>
       </c>
       <c r="Q53" s="2" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="V53">
         <f t="shared" si="4"/>
@@ -14073,7 +14073,7 @@
         <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C54">
         <v>2018</v>
@@ -14118,7 +14118,7 @@
         <v>724</v>
       </c>
       <c r="Q54" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="R54">
         <v>4.04</v>
@@ -14160,7 +14160,7 @@
         <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C55">
         <v>2018</v>
@@ -14205,7 +14205,7 @@
         <v>724</v>
       </c>
       <c r="Q55" s="2" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="R55">
         <v>3.32</v>
@@ -14247,7 +14247,7 @@
         <v>5</v>
       </c>
       <c r="B56" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C56">
         <v>2018</v>
@@ -14292,7 +14292,7 @@
         <v>724</v>
       </c>
       <c r="Q56" s="2" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="R56">
         <v>0.02</v>
@@ -14334,7 +14334,7 @@
         <v>5</v>
       </c>
       <c r="B57" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C57">
         <v>2018</v>
@@ -14379,7 +14379,7 @@
         <v>724</v>
       </c>
       <c r="Q57" s="2" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="R57">
         <v>7.0000000000000007E-2</v>
@@ -14421,7 +14421,7 @@
         <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C58">
         <v>2018</v>
@@ -14466,7 +14466,7 @@
         <v>724</v>
       </c>
       <c r="Q58" s="2" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="R58">
         <v>0.18</v>
@@ -14508,7 +14508,7 @@
         <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C59">
         <v>2018</v>
@@ -14553,7 +14553,7 @@
         <v>724</v>
       </c>
       <c r="Q59" s="2" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="R59">
         <v>0.88</v>
@@ -14595,7 +14595,7 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C60">
         <v>2017</v>
@@ -14640,7 +14640,7 @@
         <v>689</v>
       </c>
       <c r="Q60" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="R60">
         <v>2.98</v>
@@ -14682,7 +14682,7 @@
         <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C61">
         <v>2017</v>
@@ -14727,7 +14727,7 @@
         <v>689</v>
       </c>
       <c r="Q61" s="2" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="R61">
         <v>-0.64</v>
@@ -14769,7 +14769,7 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C62">
         <v>2017</v>
@@ -14814,7 +14814,7 @@
         <v>689</v>
       </c>
       <c r="Q62" s="2" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="R62">
         <v>3.49</v>
@@ -14856,7 +14856,7 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C63">
         <v>2018</v>
@@ -14889,7 +14889,7 @@
         <v>724</v>
       </c>
       <c r="Q63" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="V63">
         <v>44</v>
@@ -14921,7 +14921,7 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C64">
         <v>2016</v>
@@ -14954,7 +14954,7 @@
         <v>689</v>
       </c>
       <c r="Q64" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="V64">
         <v>177</v>
@@ -14986,7 +14986,7 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C65">
         <v>2016</v>
@@ -15019,7 +15019,7 @@
         <v>689</v>
       </c>
       <c r="Q65" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="V65">
         <v>177</v>
@@ -15051,7 +15051,7 @@
         <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C66">
         <v>2016</v>
@@ -15084,7 +15084,7 @@
         <v>689</v>
       </c>
       <c r="Q66" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="V66">
         <v>177</v>
@@ -15116,7 +15116,7 @@
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C67">
         <v>2016</v>
@@ -15203,7 +15203,7 @@
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C68">
         <v>2016</v>
@@ -15248,7 +15248,7 @@
         <v>689</v>
       </c>
       <c r="Q68" s="2" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="R68">
         <v>6.54</v>
@@ -15290,7 +15290,7 @@
         <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C69">
         <v>2016</v>
@@ -15335,7 +15335,7 @@
         <v>689</v>
       </c>
       <c r="Q69" s="2" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="R69">
         <v>0.32</v>
@@ -15377,7 +15377,7 @@
         <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C70">
         <v>2016</v>
@@ -15422,7 +15422,7 @@
         <v>689</v>
       </c>
       <c r="Q70" s="2" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="R70">
         <v>2.4</v>
@@ -15464,7 +15464,7 @@
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C71">
         <v>2016</v>
@@ -15509,7 +15509,7 @@
         <v>689</v>
       </c>
       <c r="Q71" s="2" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="R71">
         <v>7.5</v>
@@ -15551,7 +15551,7 @@
         <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C72">
         <v>2016</v>
@@ -15596,7 +15596,7 @@
         <v>689</v>
       </c>
       <c r="Q72" s="2" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="R72">
         <v>8.4</v>
@@ -15638,7 +15638,7 @@
         <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C73">
         <v>2016</v>
@@ -15683,7 +15683,7 @@
         <v>689</v>
       </c>
       <c r="Q73" s="2" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="R73">
         <v>-1.1499999999999999</v>
@@ -15725,7 +15725,7 @@
         <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C74">
         <v>2016</v>
@@ -15770,7 +15770,7 @@
         <v>689</v>
       </c>
       <c r="Q74" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="R74">
         <v>6.54</v>
@@ -15812,7 +15812,7 @@
         <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C75">
         <v>2016</v>
@@ -15857,7 +15857,7 @@
         <v>689</v>
       </c>
       <c r="Q75" s="2" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="R75">
         <v>11.5</v>
@@ -15899,7 +15899,7 @@
         <v>10</v>
       </c>
       <c r="B76" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C76">
         <v>2015</v>
@@ -15926,7 +15926,7 @@
         <v>717</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P76" t="s">
         <v>720</v>
@@ -15964,7 +15964,7 @@
         <v>11</v>
       </c>
       <c r="B77" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C77">
         <v>2015</v>
@@ -16000,7 +16000,7 @@
         <v>703</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P77" t="s">
         <v>720</v>
@@ -16047,7 +16047,7 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C78">
         <v>2014</v>
@@ -16071,7 +16071,7 @@
         <v>717</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P78" t="s">
         <v>720</v>
@@ -16109,7 +16109,7 @@
         <v>12</v>
       </c>
       <c r="B79" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C79">
         <v>2014</v>
@@ -16133,7 +16133,7 @@
         <v>717</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P79" t="s">
         <v>720</v>
@@ -16171,7 +16171,7 @@
         <v>13</v>
       </c>
       <c r="B80" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C80">
         <v>2013</v>
@@ -16204,7 +16204,7 @@
         <v>701</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P80" t="s">
         <v>720</v>
@@ -16251,7 +16251,7 @@
         <v>14</v>
       </c>
       <c r="B81" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C81">
         <v>2012</v>
@@ -16287,7 +16287,7 @@
         <v>701</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P81" t="s">
         <v>720</v>
@@ -16334,7 +16334,7 @@
         <v>15</v>
       </c>
       <c r="B82" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C82">
         <v>2012</v>
@@ -16361,7 +16361,7 @@
         <v>693</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P82" t="s">
         <v>720</v>
@@ -16399,7 +16399,7 @@
         <v>15</v>
       </c>
       <c r="B83" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C83">
         <v>2012</v>
@@ -16426,7 +16426,7 @@
         <v>693</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P83" t="s">
         <v>720</v>
@@ -16464,7 +16464,7 @@
         <v>16</v>
       </c>
       <c r="B84" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C84">
         <v>2010</v>
@@ -16509,7 +16509,7 @@
         <v>724</v>
       </c>
       <c r="Q84" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="R84">
         <v>2</v>
@@ -16551,7 +16551,7 @@
         <v>16</v>
       </c>
       <c r="B85" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C85">
         <v>2010</v>
@@ -16596,7 +16596,7 @@
         <v>724</v>
       </c>
       <c r="Q85" s="2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="R85">
         <v>-0.1</v>
@@ -16638,7 +16638,7 @@
         <v>16</v>
       </c>
       <c r="B86" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C86">
         <v>2010</v>
@@ -16683,7 +16683,7 @@
         <v>724</v>
       </c>
       <c r="Q86" s="2" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="R86">
         <v>0.39</v>
@@ -16725,7 +16725,7 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C87">
         <v>2005</v>
@@ -16761,7 +16761,7 @@
         <v>701</v>
       </c>
       <c r="O87" s="2" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P87" t="s">
         <v>720</v>
@@ -16809,7 +16809,7 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C88">
         <v>2005</v>
@@ -16851,7 +16851,7 @@
         <v>724</v>
       </c>
       <c r="Q88" s="2" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="R88">
         <v>6.54</v>
@@ -16893,7 +16893,7 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C89">
         <v>2005</v>
@@ -16935,7 +16935,7 @@
         <v>724</v>
       </c>
       <c r="Q89" s="2" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="R89">
         <v>6.39</v>
@@ -16977,7 +16977,7 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C90">
         <v>2005</v>
@@ -17019,7 +17019,7 @@
         <v>724</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="R90">
         <v>5.75</v>
@@ -17061,7 +17061,7 @@
         <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C91">
         <v>1996</v>
@@ -17148,7 +17148,7 @@
         <v>18</v>
       </c>
       <c r="B92" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C92">
         <v>1996</v>
@@ -17190,10 +17190,10 @@
         <v>748</v>
       </c>
       <c r="P92" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="Q92" s="2" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="R92">
         <v>-9.6999999999999993</v>
@@ -17235,7 +17235,7 @@
         <v>18</v>
       </c>
       <c r="B93" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C93">
         <v>1996</v>
@@ -17277,10 +17277,10 @@
         <v>748</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="Q93" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="R93">
         <v>2.9</v>
@@ -17322,7 +17322,7 @@
         <v>18</v>
       </c>
       <c r="B94" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C94">
         <v>1996</v>
@@ -17409,7 +17409,7 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C95">
         <v>1994</v>
@@ -17490,7 +17490,7 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C96">
         <v>1994</v>
@@ -17526,10 +17526,10 @@
         <v>703</v>
       </c>
       <c r="P96" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="Q96" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="R96">
         <v>3.08</v>
@@ -17571,7 +17571,7 @@
         <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C97">
         <v>1994</v>
@@ -17607,7 +17607,7 @@
         <v>703</v>
       </c>
       <c r="O97" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P97" t="s">
         <v>720</v>
@@ -17655,7 +17655,7 @@
         <v>20</v>
       </c>
       <c r="B98" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C98">
         <v>1994</v>
@@ -17685,7 +17685,7 @@
         <v>720</v>
       </c>
       <c r="Q98" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="R98">
         <v>0.13</v>
@@ -17727,7 +17727,7 @@
         <v>20</v>
       </c>
       <c r="B99" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C99">
         <v>1994</v>
@@ -17757,7 +17757,7 @@
         <v>720</v>
       </c>
       <c r="Q99" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="R99">
         <v>0.06</v>
@@ -17799,7 +17799,7 @@
         <v>20</v>
       </c>
       <c r="B100" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C100">
         <v>1994</v>
@@ -17829,7 +17829,7 @@
         <v>720</v>
       </c>
       <c r="Q100" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="R100">
         <v>1</v>
@@ -17871,7 +17871,7 @@
         <v>20</v>
       </c>
       <c r="B101" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C101">
         <v>1994</v>
@@ -17901,7 +17901,7 @@
         <v>720</v>
       </c>
       <c r="Q101" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="R101">
         <v>0.9</v>
@@ -17943,7 +17943,7 @@
         <v>20</v>
       </c>
       <c r="B102" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C102">
         <v>1994</v>
@@ -17973,7 +17973,7 @@
         <v>720</v>
       </c>
       <c r="Q102" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="R102">
         <v>0.6</v>
@@ -18015,7 +18015,7 @@
         <v>20</v>
       </c>
       <c r="B103" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C103">
         <v>1994</v>
@@ -18045,7 +18045,7 @@
         <v>720</v>
       </c>
       <c r="Q103" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="R103">
         <v>0.7</v>
@@ -18087,7 +18087,7 @@
         <v>20</v>
       </c>
       <c r="B104" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C104">
         <v>1994</v>
@@ -18117,7 +18117,7 @@
         <v>720</v>
       </c>
       <c r="Q104" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="R104">
         <v>0.5</v>
@@ -18159,7 +18159,7 @@
         <v>20</v>
       </c>
       <c r="B105" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C105">
         <v>1994</v>
@@ -18189,7 +18189,7 @@
         <v>720</v>
       </c>
       <c r="Q105" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="R105">
         <v>0.7</v>
@@ -18231,7 +18231,7 @@
         <v>21</v>
       </c>
       <c r="B106" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C106">
         <v>1994</v>
@@ -18315,7 +18315,7 @@
         <v>21</v>
       </c>
       <c r="B107" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C107">
         <v>1994</v>
@@ -18399,10 +18399,10 @@
         <v>22</v>
       </c>
       <c r="B108" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C108" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D108">
         <v>107</v>
@@ -18432,7 +18432,7 @@
         <v>724</v>
       </c>
       <c r="Q108" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="R108">
         <v>0.1716</v>
@@ -18474,10 +18474,10 @@
         <v>22</v>
       </c>
       <c r="B109" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C109" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D109">
         <v>108</v>
@@ -18549,10 +18549,10 @@
         <v>22</v>
       </c>
       <c r="B110" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C110" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D110">
         <v>109</v>
@@ -18579,10 +18579,10 @@
         <v>735</v>
       </c>
       <c r="P110" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="Q110" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="R110">
         <v>-2.4024000000000001</v>
@@ -18624,10 +18624,10 @@
         <v>22</v>
       </c>
       <c r="B111" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C111" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D111">
         <v>110</v>
@@ -18657,7 +18657,7 @@
         <v>704</v>
       </c>
       <c r="Q111" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="R111">
         <v>1.2333000000000001</v>
@@ -18699,10 +18699,10 @@
         <v>22</v>
       </c>
       <c r="B112" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C112" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D112">
         <v>111</v>
@@ -18732,7 +18732,7 @@
         <v>704</v>
       </c>
       <c r="Q112" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="R112">
         <v>9.7385000000000002</v>
@@ -18774,10 +18774,10 @@
         <v>23</v>
       </c>
       <c r="B113" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C113" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D113">
         <v>112</v>
@@ -18807,7 +18807,7 @@
         <v>704</v>
       </c>
       <c r="Q113" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="R113">
         <v>14.4582555</v>
@@ -18849,10 +18849,10 @@
         <v>23</v>
       </c>
       <c r="B114" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C114" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D114">
         <v>113</v>
@@ -18882,7 +18882,7 @@
         <v>704</v>
       </c>
       <c r="Q114" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="R114">
         <v>16.5448789</v>
@@ -18924,10 +18924,10 @@
         <v>23</v>
       </c>
       <c r="B115" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C115" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D115">
         <v>114</v>
@@ -19017,133 +19017,133 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>708</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
+        <v>824</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>825</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>826</v>
-      </c>
       <c r="C2" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
+        <v>826</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>827</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>828</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="8" t="s">
+        <v>828</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>829</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>830</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>831</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>832</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>833</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>834</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>835</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>836</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>836</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>837</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>838</v>
-      </c>
       <c r="C8" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>838</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>839</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>840</v>
-      </c>
       <c r="C9" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>840</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>841</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>842</v>
-      </c>
       <c r="C10" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
   </sheetData>
@@ -19163,21 +19163,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F3729CDE7EAEF44A53FFF2D231E047F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fa77f95735d7b1684a0f9f1d46cbd95">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2efe24bd-a7c1-481d-a426-3119fcfe7149" xmlns:ns4="061b3361-47e6-4fd1-b7fc-4e45b1c77d33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9154525a1bae266bab7d07ed10795e6b" ns3:_="" ns4:_="">
     <xsd:import namespace="2efe24bd-a7c1-481d-a426-3119fcfe7149"/>
@@ -19400,10 +19385,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E891FD6-EDA9-457E-8FC4-26FFD11BC970}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F22CBBB-A5A9-4CD6-A22C-EA1A13EBE8FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2efe24bd-a7c1-481d-a426-3119fcfe7149"/>
+    <ds:schemaRef ds:uri="061b3361-47e6-4fd1-b7fc-4e45b1c77d33"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19426,20 +19437,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F22CBBB-A5A9-4CD6-A22C-EA1A13EBE8FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E891FD6-EDA9-457E-8FC4-26FFD11BC970}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2efe24bd-a7c1-481d-a426-3119fcfe7149"/>
-    <ds:schemaRef ds:uri="061b3361-47e6-4fd1-b7fc-4e45b1c77d33"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Begun new analyses. Updated pubmed search
</commit_message>
<xml_diff>
--- a/meta_spreadsheet.xlsx
+++ b/meta_spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fsu-my.sharepoint.com/personal/ajg17d_fsu_edu/Documents/Florida State University/Research Projects/meta_suicide_erp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajg17d\OneDrive - Florida State University\Florida State University\Research Projects\meta_suicide_erp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1084" documentId="8_{AE6EE886-186C-438A-A3D8-7543467F2F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{09BEBDD4-7CA1-4F87-B6DA-D60AA999306C}"/>
+  <xr:revisionPtr revIDLastSave="1089" documentId="8_{AE6EE886-186C-438A-A3D8-7543467F2F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{988859FB-D83D-457E-9418-C0D7AB3BABF0}"/>
   <bookViews>
-    <workbookView xWindow="353" yWindow="3600" windowWidth="4282" windowHeight="8287" firstSheet="2" activeTab="2" xr2:uid="{FF3FF6FC-0C5E-41B5-84E2-C5FF2C3F66C7}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{FF3FF6FC-0C5E-41B5-84E2-C5FF2C3F66C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3163" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3165" uniqueCount="971">
   <si>
     <t>Database</t>
   </si>
@@ -2944,6 +2944,12 @@
   </si>
   <si>
     <t>diff</t>
+  </si>
+  <si>
+    <t>Date2</t>
+  </si>
+  <si>
+    <t># New</t>
   </si>
 </sst>
 </file>
@@ -4394,19 +4400,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C14CA69-90BD-40F0-91ED-5F03B1240544}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4419,8 +4426,14 @@
       <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -4433,8 +4446,14 @@
       <c r="D2">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" s="3">
+        <v>44120</v>
+      </c>
+      <c r="F2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -4448,7 +4467,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4462,7 +4481,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4476,7 +4495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <f>SUM(D2:D5)</f>
         <v>270</v>
@@ -4496,14 +4515,14 @@
       <selection activeCell="D151" sqref="D151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -4526,7 +4545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -4549,7 +4568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -4572,7 +4591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -4595,7 +4614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -4618,7 +4637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -4641,7 +4660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -4664,7 +4683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -4687,7 +4706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -4710,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -4733,7 +4752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -4753,7 +4772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -4776,7 +4795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -4799,7 +4818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -4822,7 +4841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>88</v>
       </c>
@@ -4845,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -4868,7 +4887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -4891,7 +4910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -4914,7 +4933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>95</v>
       </c>
@@ -4937,7 +4956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>96</v>
       </c>
@@ -4960,7 +4979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -4983,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -5006,7 +5025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -5029,7 +5048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>104</v>
       </c>
@@ -5052,7 +5071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -5075,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -5098,7 +5117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -5121,7 +5140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>111</v>
       </c>
@@ -5144,7 +5163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>116</v>
       </c>
@@ -5167,7 +5186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>121</v>
       </c>
@@ -5190,7 +5209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>125</v>
       </c>
@@ -5213,7 +5232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>136</v>
       </c>
@@ -5236,7 +5255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -5259,7 +5278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -5282,7 +5301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>151</v>
       </c>
@@ -5305,7 +5324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>168</v>
       </c>
@@ -5328,7 +5347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>171</v>
       </c>
@@ -5348,7 +5367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>661</v>
       </c>
@@ -5371,7 +5390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>184</v>
       </c>
@@ -5391,7 +5410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>684</v>
       </c>
@@ -5414,7 +5433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>521</v>
       </c>
@@ -5437,7 +5456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>543</v>
       </c>
@@ -5460,7 +5479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>578</v>
       </c>
@@ -5483,7 +5502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>584</v>
       </c>
@@ -5506,7 +5525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>644</v>
       </c>
@@ -5529,7 +5548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>647</v>
       </c>
@@ -5552,7 +5571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>663</v>
       </c>
@@ -5572,7 +5591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>666</v>
       </c>
@@ -5592,7 +5611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>670</v>
       </c>
@@ -5612,7 +5631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>672</v>
       </c>
@@ -5632,7 +5651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>675</v>
       </c>
@@ -5652,7 +5671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -5675,7 +5694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -5698,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>46</v>
       </c>
@@ -5721,7 +5740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -5744,7 +5763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -5767,7 +5786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -5790,7 +5809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -5813,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -5836,7 +5855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>67</v>
       </c>
@@ -5859,7 +5878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>68</v>
       </c>
@@ -5882,7 +5901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>69</v>
       </c>
@@ -5905,7 +5924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -5928,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -5951,7 +5970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -5974,7 +5993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>75</v>
       </c>
@@ -5997,7 +6016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -6020,7 +6039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -6043,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -6060,7 +6079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -6083,7 +6102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>80</v>
       </c>
@@ -6106,7 +6125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -6129,7 +6148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>83</v>
       </c>
@@ -6152,7 +6171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -6175,7 +6194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -6198,7 +6217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>89</v>
       </c>
@@ -6218,7 +6237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>91</v>
       </c>
@@ -6241,7 +6260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>94</v>
       </c>
@@ -6264,7 +6283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>98</v>
       </c>
@@ -6287,7 +6306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>99</v>
       </c>
@@ -6310,7 +6329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>101</v>
       </c>
@@ -6333,7 +6352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>102</v>
       </c>
@@ -6356,7 +6375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>105</v>
       </c>
@@ -6379,7 +6398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>109</v>
       </c>
@@ -6402,7 +6421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>110</v>
       </c>
@@ -6425,7 +6444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>112</v>
       </c>
@@ -6448,7 +6467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>113</v>
       </c>
@@ -6471,7 +6490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>114</v>
       </c>
@@ -6494,7 +6513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>115</v>
       </c>
@@ -6517,7 +6536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>117</v>
       </c>
@@ -6537,7 +6556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>118</v>
       </c>
@@ -6560,7 +6579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>119</v>
       </c>
@@ -6580,7 +6599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>120</v>
       </c>
@@ -6603,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>122</v>
       </c>
@@ -6626,7 +6645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>123</v>
       </c>
@@ -6649,7 +6668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>124</v>
       </c>
@@ -6672,7 +6691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>126</v>
       </c>
@@ -6695,7 +6714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>127</v>
       </c>
@@ -6718,7 +6737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>128</v>
       </c>
@@ -6741,7 +6760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>129</v>
       </c>
@@ -6764,7 +6783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>130</v>
       </c>
@@ -6787,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>131</v>
       </c>
@@ -6810,7 +6829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>132</v>
       </c>
@@ -6833,7 +6852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>133</v>
       </c>
@@ -6856,7 +6875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>134</v>
       </c>
@@ -6879,7 +6898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>135</v>
       </c>
@@ -6902,7 +6921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>137</v>
       </c>
@@ -6925,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>138</v>
       </c>
@@ -6948,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>139</v>
       </c>
@@ -6971,7 +6990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>140</v>
       </c>
@@ -6994,7 +7013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>141</v>
       </c>
@@ -7017,7 +7036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>142</v>
       </c>
@@ -7040,7 +7059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>143</v>
       </c>
@@ -7063,7 +7082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>144</v>
       </c>
@@ -7086,7 +7105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>146</v>
       </c>
@@ -7106,7 +7125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>147</v>
       </c>
@@ -7129,7 +7148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>148</v>
       </c>
@@ -7152,7 +7171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>150</v>
       </c>
@@ -7175,7 +7194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>152</v>
       </c>
@@ -7198,7 +7217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>153</v>
       </c>
@@ -7221,7 +7240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>154</v>
       </c>
@@ -7244,7 +7263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>155</v>
       </c>
@@ -7267,7 +7286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>156</v>
       </c>
@@ -7290,7 +7309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>157</v>
       </c>
@@ -7310,7 +7329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>158</v>
       </c>
@@ -7333,7 +7352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>159</v>
       </c>
@@ -7356,7 +7375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>160</v>
       </c>
@@ -7379,7 +7398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>161</v>
       </c>
@@ -7402,7 +7421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>162</v>
       </c>
@@ -7425,7 +7444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>163</v>
       </c>
@@ -7448,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>164</v>
       </c>
@@ -7471,7 +7490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>165</v>
       </c>
@@ -7491,7 +7510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>166</v>
       </c>
@@ -7511,7 +7530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>167</v>
       </c>
@@ -7534,7 +7553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>169</v>
       </c>
@@ -7557,7 +7576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>170</v>
       </c>
@@ -7577,7 +7596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>172</v>
       </c>
@@ -7597,7 +7616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>173</v>
       </c>
@@ -7620,7 +7639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>174</v>
       </c>
@@ -7643,7 +7662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>175</v>
       </c>
@@ -7666,7 +7685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>176</v>
       </c>
@@ -7689,7 +7708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>177</v>
       </c>
@@ -7712,7 +7731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>178</v>
       </c>
@@ -7735,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>179</v>
       </c>
@@ -7758,7 +7777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>180</v>
       </c>
@@ -7781,7 +7800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>181</v>
       </c>
@@ -7804,7 +7823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>182</v>
       </c>
@@ -7827,7 +7846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>183</v>
       </c>
@@ -7847,7 +7866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>185</v>
       </c>
@@ -7870,7 +7889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>186</v>
       </c>
@@ -7893,7 +7912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>187</v>
       </c>
@@ -7913,7 +7932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>188</v>
       </c>
@@ -7933,7 +7952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>189</v>
       </c>
@@ -7953,7 +7972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>190</v>
       </c>
@@ -7973,7 +7992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>191</v>
       </c>
@@ -7993,7 +8012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>59</v>
       </c>
@@ -8016,7 +8035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>537</v>
       </c>
@@ -8036,7 +8055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>539</v>
       </c>
@@ -8059,7 +8078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>565</v>
       </c>
@@ -8082,7 +8101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>555</v>
       </c>
@@ -8105,7 +8124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>527</v>
       </c>
@@ -8128,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>523</v>
       </c>
@@ -8151,7 +8170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>566</v>
       </c>
@@ -8171,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>559</v>
       </c>
@@ -8194,7 +8213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>547</v>
       </c>
@@ -8217,7 +8236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>558</v>
       </c>
@@ -8240,7 +8259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>533</v>
       </c>
@@ -8263,7 +8282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>129</v>
       </c>
@@ -8286,7 +8305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>551</v>
       </c>
@@ -8306,7 +8325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>567</v>
       </c>
@@ -8329,7 +8348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>571</v>
       </c>
@@ -8352,7 +8371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>574</v>
       </c>
@@ -8375,7 +8394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>581</v>
       </c>
@@ -8395,7 +8414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>588</v>
       </c>
@@ -8418,7 +8437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>592</v>
       </c>
@@ -8438,7 +8457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>594</v>
       </c>
@@ -8458,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>597</v>
       </c>
@@ -8478,7 +8497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>600</v>
       </c>
@@ -8501,7 +8520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>604</v>
       </c>
@@ -8524,7 +8543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>608</v>
       </c>
@@ -8547,7 +8566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>611</v>
       </c>
@@ -8567,7 +8586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>613</v>
       </c>
@@ -8587,7 +8606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>615</v>
       </c>
@@ -8610,7 +8629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>619</v>
       </c>
@@ -8633,7 +8652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>622</v>
       </c>
@@ -8656,7 +8675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>625</v>
       </c>
@@ -8679,7 +8698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>628</v>
       </c>
@@ -8699,7 +8718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>630</v>
       </c>
@@ -8722,7 +8741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>634</v>
       </c>
@@ -8745,7 +8764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>637</v>
       </c>
@@ -8768,7 +8787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>651</v>
       </c>
@@ -8791,7 +8810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>655</v>
       </c>
@@ -8814,7 +8833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>656</v>
       </c>
@@ -8837,7 +8856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>659</v>
       </c>
@@ -8857,7 +8876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>678</v>
       </c>
@@ -8877,7 +8896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>681</v>
       </c>
@@ -8897,7 +8916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G197">
         <f>SUM(G2:G196)</f>
         <v>46</v>
@@ -8917,27 +8936,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E9CFB2-E36F-473E-93F7-18105F56F26D}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.59765625" customWidth="1"/>
-    <col min="15" max="15" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -8987,7 +9006,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9025,7 +9044,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -9063,7 +9082,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -9101,7 +9120,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>684</v>
       </c>
@@ -9139,7 +9158,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -9171,7 +9190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -9203,7 +9222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>64</v>
       </c>
@@ -9232,7 +9251,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -9264,7 +9283,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -9302,7 +9321,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -9340,7 +9359,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -9369,7 +9388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>521</v>
       </c>
@@ -9407,7 +9426,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>82</v>
       </c>
@@ -9439,7 +9458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -9471,7 +9490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -9509,7 +9528,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -9547,7 +9566,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -9579,7 +9598,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -9617,7 +9636,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -9655,7 +9674,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>644</v>
       </c>
@@ -9684,7 +9703,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>647</v>
       </c>
@@ -9713,7 +9732,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>95</v>
       </c>
@@ -9760,7 +9779,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>96</v>
       </c>
@@ -9801,7 +9820,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>97</v>
       </c>
@@ -9833,7 +9852,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -9865,7 +9884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>103</v>
       </c>
@@ -9897,7 +9916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -9935,7 +9954,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>106</v>
       </c>
@@ -9973,7 +9992,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>107</v>
       </c>
@@ -10011,7 +10030,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>108</v>
       </c>
@@ -10049,7 +10068,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>663</v>
       </c>
@@ -10084,7 +10103,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>111</v>
       </c>
@@ -10122,7 +10141,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>666</v>
       </c>
@@ -10145,7 +10164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>116</v>
       </c>
@@ -10183,7 +10202,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>672</v>
       </c>
@@ -10212,7 +10231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>121</v>
       </c>
@@ -10244,7 +10263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>125</v>
       </c>
@@ -10270,7 +10289,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -10305,7 +10324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -10346,7 +10365,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>149</v>
       </c>
@@ -10387,7 +10406,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -10428,7 +10447,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>578</v>
       </c>
@@ -10463,7 +10482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>584</v>
       </c>
@@ -10498,7 +10517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>675</v>
       </c>
@@ -10521,7 +10540,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>168</v>
       </c>
@@ -10556,7 +10575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>171</v>
       </c>
@@ -10588,7 +10607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>842</v>
       </c>
@@ -10629,7 +10648,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>845</v>
       </c>
@@ -10664,7 +10683,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>44</v>
       </c>
@@ -10693,7 +10712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>44</v>
       </c>
@@ -10722,7 +10741,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>195</v>
       </c>
@@ -10767,29 +10786,29 @@
       <selection pane="topRight" activeCell="W77" sqref="W77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.265625" customWidth="1"/>
-    <col min="5" max="5" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.3984375" customWidth="1"/>
-    <col min="7" max="7" width="10.3984375" customWidth="1"/>
-    <col min="8" max="8" width="10.1328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="12.265625" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.28515625" customWidth="1"/>
     <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="6.73046875" customWidth="1"/>
-    <col min="26" max="26" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="6.7109375" customWidth="1"/>
+    <col min="26" max="26" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -10887,7 +10906,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -10955,7 +10974,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -11023,7 +11042,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11091,7 +11110,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -11159,7 +11178,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -11227,7 +11246,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -11295,7 +11314,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -11363,7 +11382,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -11431,7 +11450,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -11499,7 +11518,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -11567,7 +11586,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -11635,7 +11654,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -11703,7 +11722,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -11771,7 +11790,7 @@
         <v>1.9877613749829152E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -11861,7 +11880,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -11951,7 +11970,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -12041,7 +12060,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -12131,7 +12150,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -12221,7 +12240,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -12311,7 +12330,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -12401,7 +12420,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -12491,7 +12510,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -12581,7 +12600,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -12671,7 +12690,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -12761,7 +12780,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -12851,7 +12870,7 @@
         <v>6.8412149951567913E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -12919,7 +12938,7 @@
         <v>0.28196343969713361</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -12987,7 +13006,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3</v>
       </c>
@@ -13055,7 +13074,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -13123,7 +13142,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3</v>
       </c>
@@ -13191,7 +13210,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -13259,7 +13278,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -13327,7 +13346,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -13395,7 +13414,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -13463,7 +13482,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -13531,7 +13550,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -13599,7 +13618,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -13667,7 +13686,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -13735,7 +13754,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -13803,7 +13822,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -13871,7 +13890,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -13939,7 +13958,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -14007,7 +14026,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -14075,7 +14094,7 @@
         <v>6.8060140616549497E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -14143,7 +14162,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -14211,7 +14230,7 @@
         <v>8.750589507842077E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -14279,7 +14298,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -14347,7 +14366,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -14415,7 +14434,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>3</v>
       </c>
@@ -14483,7 +14502,7 @@
         <v>7.7783017847485134E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -14564,7 +14583,7 @@
         <v>6.843580356015655E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>4</v>
       </c>
@@ -14654,7 +14673,7 @@
         <v>6.843580356015655E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4</v>
       </c>
@@ -14735,7 +14754,7 @@
         <v>6.843580356015655E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5</v>
       </c>
@@ -14825,7 +14844,7 @@
         <v>0.18644470868014273</v>
       </c>
     </row>
-    <row r="55" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5</v>
       </c>
@@ -14915,7 +14934,7 @@
         <v>0.15847800237812132</v>
       </c>
     </row>
-    <row r="56" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5</v>
       </c>
@@ -15005,7 +15024,7 @@
         <v>0.15847800237812132</v>
       </c>
     </row>
-    <row r="57" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5</v>
       </c>
@@ -15095,7 +15114,7 @@
         <v>0.15847800237812132</v>
       </c>
     </row>
-    <row r="58" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5</v>
       </c>
@@ -15185,7 +15204,7 @@
         <v>0.16780023781212844</v>
       </c>
     </row>
-    <row r="59" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5</v>
       </c>
@@ -15275,7 +15294,7 @@
         <v>0.15847800237812132</v>
       </c>
     </row>
-    <row r="60" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>6</v>
       </c>
@@ -15365,7 +15384,7 @@
         <v>1.9871314006975397E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>6</v>
       </c>
@@ -15455,7 +15474,7 @@
         <v>1.9871314006975397E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>6</v>
       </c>
@@ -15545,7 +15564,7 @@
         <v>1.9871314006975397E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7</v>
       </c>
@@ -15613,7 +15632,7 @@
         <v>9.6439456416508307E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>8</v>
       </c>
@@ -15681,7 +15700,7 @@
         <v>1.9828694579012325E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>8</v>
       </c>
@@ -15749,7 +15768,7 @@
         <v>1.9828694579012325E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>8</v>
       </c>
@@ -15817,7 +15836,7 @@
         <v>1.9828694579012325E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9</v>
       </c>
@@ -15907,7 +15926,7 @@
         <v>0.14277215942891133</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9</v>
       </c>
@@ -15997,7 +16016,7 @@
         <v>0.14277215942891133</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9</v>
       </c>
@@ -16087,7 +16106,7 @@
         <v>0.14277215942891133</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9</v>
       </c>
@@ -16177,7 +16196,7 @@
         <v>0.13325401546698393</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9</v>
       </c>
@@ -16267,7 +16286,7 @@
         <v>0.13325401546698393</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9</v>
       </c>
@@ -16357,7 +16376,7 @@
         <v>0.13325401546698393</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9</v>
       </c>
@@ -16447,7 +16466,7 @@
         <v>0.14277215942891133</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9</v>
       </c>
@@ -16537,7 +16556,7 @@
         <v>0.13325401546698393</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9</v>
       </c>
@@ -16627,7 +16646,7 @@
         <v>0.15229030339083877</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>10</v>
       </c>
@@ -16695,7 +16714,7 @@
         <v>0.1057831425598335</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>11</v>
       </c>
@@ -16781,7 +16800,7 @@
         <v>9.6065962019209694E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>12</v>
       </c>
@@ -16846,7 +16865,7 @@
         <v>8.7359557378242622E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>12</v>
       </c>
@@ -16911,7 +16930,7 @@
         <v>5.8638985672772481E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>13</v>
       </c>
@@ -16994,7 +17013,7 @@
         <v>0.10543302850995159</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>14</v>
       </c>
@@ -17080,7 +17099,7 @@
         <v>9.8937120033820339E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>15</v>
       </c>
@@ -17148,7 +17167,7 @@
         <v>9.6166493236212278E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>15</v>
       </c>
@@ -17216,7 +17235,7 @@
         <v>9.6166493236212278E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>16</v>
       </c>
@@ -17306,7 +17325,7 @@
         <v>0.21314328006359476</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>16</v>
       </c>
@@ -17396,7 +17415,7 @@
         <v>8.7194978207834214E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>16</v>
       </c>
@@ -17486,7 +17505,7 @@
         <v>8.7194978207834214E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>17</v>
       </c>
@@ -17573,7 +17592,7 @@
         <v>8.7894809688581321E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>17</v>
       </c>
@@ -17660,7 +17679,7 @@
         <v>8.7894809688581321E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>17</v>
       </c>
@@ -17747,7 +17766,7 @@
         <v>7.8128719723183401E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>17</v>
       </c>
@@ -17834,7 +17853,7 @@
         <v>7.8128719723183401E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>18</v>
       </c>
@@ -17924,7 +17943,7 @@
         <v>0.28435627851616746</v>
       </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>18</v>
       </c>
@@ -18014,7 +18033,7 @@
         <v>0.18345566355881771</v>
       </c>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>18</v>
       </c>
@@ -18104,7 +18123,7 @@
         <v>0.32104741122793096</v>
       </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>18</v>
       </c>
@@ -18194,7 +18213,7 @@
         <v>0.21097401309264038</v>
       </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>19</v>
       </c>
@@ -18278,7 +18297,7 @@
         <v>5.861808857947854E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>19</v>
       </c>
@@ -18362,7 +18381,7 @@
         <v>5.861808857947854E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>19</v>
       </c>
@@ -18449,7 +18468,7 @@
         <v>5.861808857947854E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>20</v>
       </c>
@@ -18524,7 +18543,7 @@
         <v>0.16832749667914504</v>
       </c>
     </row>
-    <row r="99" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>20</v>
       </c>
@@ -18599,7 +18618,7 @@
         <v>0.1589759690858592</v>
       </c>
     </row>
-    <row r="100" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>20</v>
       </c>
@@ -18674,7 +18693,7 @@
         <v>0.20360839609037015</v>
       </c>
     </row>
-    <row r="101" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>20</v>
       </c>
@@ -18749,7 +18768,7 @@
         <v>0.19435346899535333</v>
       </c>
     </row>
-    <row r="102" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>20</v>
       </c>
@@ -18824,7 +18843,7 @@
         <v>0.20360839609037015</v>
       </c>
     </row>
-    <row r="103" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>20</v>
       </c>
@@ -18899,7 +18918,7 @@
         <v>0.30286641427798805</v>
       </c>
     </row>
-    <row r="104" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>20</v>
       </c>
@@ -18974,7 +18993,7 @@
         <v>0.31151974040021629</v>
       </c>
     </row>
-    <row r="105" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>20</v>
       </c>
@@ -19049,7 +19068,7 @@
         <v>0.35478637101135746</v>
       </c>
     </row>
-    <row r="106" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>21</v>
       </c>
@@ -19136,7 +19155,7 @@
         <v>0.31550928021729291</v>
       </c>
     </row>
-    <row r="107" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>21</v>
       </c>
@@ -19223,7 +19242,7 @@
         <v>0.30674513354459032</v>
       </c>
     </row>
-    <row r="108" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>22</v>
       </c>
@@ -19301,7 +19320,7 @@
         <v>6.8193624557260926E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>22</v>
       </c>
@@ -19379,7 +19398,7 @@
         <v>6.8193624557260926E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>22</v>
       </c>
@@ -19457,7 +19476,7 @@
         <v>6.8193624557260926E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>22</v>
       </c>
@@ -19535,7 +19554,7 @@
         <v>6.8193624557260926E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>22</v>
       </c>
@@ -19610,7 +19629,7 @@
         <v>6.8193624557260926E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>23</v>
       </c>
@@ -19688,7 +19707,7 @@
         <v>7.755739644970415E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>23</v>
       </c>
@@ -19766,7 +19785,7 @@
         <v>7.755739644970415E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>23</v>
       </c>
@@ -19844,7 +19863,7 @@
         <v>7.755739644970415E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>24</v>
       </c>
@@ -19900,7 +19919,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>24</v>
       </c>
@@ -19956,7 +19975,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>24</v>
       </c>
@@ -20012,7 +20031,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>24</v>
       </c>
@@ -20068,7 +20087,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>24</v>
       </c>
@@ -20124,7 +20143,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>24</v>
       </c>
@@ -20180,7 +20199,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>24</v>
       </c>
@@ -20236,7 +20255,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>24</v>
       </c>
@@ -20292,7 +20311,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>24</v>
       </c>
@@ -20348,7 +20367,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>24</v>
       </c>
@@ -20404,7 +20423,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>24</v>
       </c>
@@ -20460,7 +20479,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>24</v>
       </c>
@@ -20516,7 +20535,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>24</v>
       </c>
@@ -20572,7 +20591,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>24</v>
       </c>
@@ -20628,7 +20647,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>24</v>
       </c>
@@ -20684,7 +20703,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>24</v>
       </c>
@@ -20740,7 +20759,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>24</v>
       </c>
@@ -20796,7 +20815,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>24</v>
       </c>
@@ -20852,7 +20871,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>24</v>
       </c>
@@ -20908,7 +20927,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>24</v>
       </c>
@@ -20964,7 +20983,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>24</v>
       </c>
@@ -21020,7 +21039,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>24</v>
       </c>
@@ -21076,7 +21095,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>24</v>
       </c>
@@ -21132,7 +21151,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>24</v>
       </c>
@@ -21188,7 +21207,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>24</v>
       </c>
@@ -21244,7 +21263,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>24</v>
       </c>
@@ -21300,7 +21319,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>24</v>
       </c>
@@ -21356,7 +21375,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>24</v>
       </c>
@@ -21412,7 +21431,7 @@
         <v>4.9118959981204482E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>24</v>
       </c>
@@ -21468,7 +21487,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>24</v>
       </c>
@@ -21524,7 +21543,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>24</v>
       </c>
@@ -21580,7 +21599,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>24</v>
       </c>
@@ -21636,7 +21655,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>24</v>
       </c>
@@ -21692,7 +21711,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>24</v>
       </c>
@@ -21748,7 +21767,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>24</v>
       </c>
@@ -21804,7 +21823,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>24</v>
       </c>
@@ -21860,7 +21879,7 @@
         <v>4.9108487413677883E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>24</v>
       </c>
@@ -21916,7 +21935,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>24</v>
       </c>
@@ -21972,7 +21991,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>24</v>
       </c>
@@ -22028,7 +22047,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>24</v>
       </c>
@@ -22084,7 +22103,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>24</v>
       </c>
@@ -22140,7 +22159,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>24</v>
       </c>
@@ -22196,7 +22215,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>24</v>
       </c>
@@ -22252,7 +22271,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>24</v>
       </c>
@@ -22308,7 +22327,7 @@
         <v>3.9319161370443424E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>24</v>
       </c>
@@ -22364,7 +22383,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>24</v>
       </c>
@@ -22420,7 +22439,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>24</v>
       </c>
@@ -22476,7 +22495,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>24</v>
       </c>
@@ -22532,7 +22551,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>24</v>
       </c>
@@ -22588,7 +22607,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>24</v>
       </c>
@@ -22644,7 +22663,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>24</v>
       </c>
@@ -22700,7 +22719,7 @@
         <v>4.9158500297560012E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>24</v>
       </c>
@@ -22756,7 +22775,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>24</v>
       </c>
@@ -22812,7 +22831,7 @@
         <v>3.9319161370443424E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>24</v>
       </c>
@@ -22868,7 +22887,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>24</v>
       </c>
@@ -22924,7 +22943,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>24</v>
       </c>
@@ -22980,7 +22999,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>24</v>
       </c>
@@ -23036,7 +23055,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>24</v>
       </c>
@@ -23092,7 +23111,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>24</v>
       </c>
@@ -23148,7 +23167,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>24</v>
       </c>
@@ -23204,7 +23223,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>24</v>
       </c>
@@ -23260,7 +23279,7 @@
         <v>3.9319161370443424E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>24</v>
       </c>
@@ -23316,7 +23335,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>24</v>
       </c>
@@ -23372,7 +23391,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>24</v>
       </c>
@@ -23428,7 +23447,7 @@
         <v>4.9158500297560012E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>24</v>
       </c>
@@ -23484,7 +23503,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>24</v>
       </c>
@@ -23540,7 +23559,7 @@
         <v>3.9326800238048007E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>24</v>
       </c>
@@ -23596,7 +23615,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>24</v>
       </c>
@@ -23652,7 +23671,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>24</v>
       </c>
@@ -23708,7 +23727,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>24</v>
       </c>
@@ -23764,7 +23783,7 @@
         <v>4.9148951713054279E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>24</v>
       </c>
@@ -23820,7 +23839,7 @@
         <v>3.9319161370443424E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>24</v>
       </c>
@@ -23876,7 +23895,7 @@
         <v>3.9319161370443424E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>24</v>
       </c>
@@ -23932,7 +23951,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>24</v>
       </c>
@@ -23988,7 +24007,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>24</v>
       </c>
@@ -24044,7 +24063,7 @@
         <v>4.9129189368375431E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>24</v>
       </c>
@@ -24100,7 +24119,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>24</v>
       </c>
@@ -24156,7 +24175,7 @@
         <v>4.9139183948043751E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>24</v>
       </c>
@@ -24228,13 +24247,13 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>820</v>
       </c>
@@ -24248,7 +24267,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>821</v>
       </c>
@@ -24262,7 +24281,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>823</v>
       </c>
@@ -24276,7 +24295,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>825</v>
       </c>
@@ -24290,7 +24309,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>827</v>
       </c>
@@ -24304,7 +24323,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>829</v>
       </c>
@@ -24318,7 +24337,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>831</v>
       </c>
@@ -24332,7 +24351,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>833</v>
       </c>
@@ -24343,7 +24362,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>835</v>
       </c>
@@ -24354,7 +24373,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>837</v>
       </c>
@@ -24365,7 +24384,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>966</v>
       </c>
@@ -24376,7 +24395,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>967</v>
       </c>
@@ -24404,6 +24423,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009F3729CDE7EAEF44A53FFF2D231E047F" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1fa77f95735d7b1684a0f9f1d46cbd95">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2efe24bd-a7c1-481d-a426-3119fcfe7149" xmlns:ns4="061b3361-47e6-4fd1-b7fc-4e45b1c77d33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9154525a1bae266bab7d07ed10795e6b" ns3:_="" ns4:_="">
     <xsd:import namespace="2efe24bd-a7c1-481d-a426-3119fcfe7149"/>
@@ -24626,22 +24654,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E891FD6-EDA9-457E-8FC4-26FFD11BC970}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F22CBBB-A5A9-4CD6-A22C-EA1A13EBE8FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24660,7 +24687,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1B9A47D-9A6D-4087-8FA8-4E1598E50986}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -24675,12 +24702,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E891FD6-EDA9-457E-8FC4-26FFD11BC970}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>